<commit_message>
Created Added Link Parsing
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="284">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -593,7 +593,10 @@
     <t>9284K616</t>
   </si>
   <si>
-    <t>Polyester Expandable Sleeving 10'</t>
+    <t>Polyester Expandable Sleeving</t>
+  </si>
+  <si>
+    <t>10ft</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/9284K616-9284K364/</t>
@@ -602,7 +605,10 @@
     <t>5549K37</t>
   </si>
   <si>
-    <t>Abrasion-Resistant Versilon Polyurethane Tubing 5'</t>
+    <t>Abrasion-Resistant Versilon Polyurethane Tubing</t>
+  </si>
+  <si>
+    <t>5ft</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/5549K37/</t>
@@ -611,7 +617,7 @@
     <t>5234K52-5234K82</t>
   </si>
   <si>
-    <t>Super-Soft Latex Rubber Tubing for Air&amp;Water 5'</t>
+    <t>Super-Soft Latex Rubber Tubing for Air&amp;Water</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/5234K52-5234K82/</t>
@@ -650,7 +656,7 @@
     <t>5108K58</t>
   </si>
   <si>
-    <t>Abrasion-Resistant Polyurethane Tube for Air 10'</t>
+    <t>Abrasion-Resistant Polyurethane Tube for Air</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/5108K58/</t>
@@ -686,6 +692,9 @@
     <t>Worm Drive Clamps</t>
   </si>
   <si>
+    <t>2 packs</t>
+  </si>
+  <si>
     <t>https://www.mcmaster.com/5011T171/</t>
   </si>
   <si>
@@ -704,7 +713,7 @@
     <t>16 Channel Relay Board</t>
   </si>
   <si>
-    <t>Amazon.com: D-FLIFE 5V 16-Channel Relay Interface Board Module Optocoupler LED LM2576 Power for Arduino DIY Kit PiC ARM AVR (5V 16-Channel) : Electronics</t>
+    <t>https://www.amazon.com/D-FLIFE-16-Channel-Interface-Optocoupler-Arduino/dp/B09534Y25Z/ref=asc_df_B09534Y25Z/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=532825377821&amp;hvpos=&amp;hvnetw=g&amp;hvrand=14483958407250822251&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9005677&amp;hvtargid=pla-1581279485192&amp;psc=1</t>
   </si>
   <si>
     <t>4089K61-4089K15</t>
@@ -749,6 +758,9 @@
     <t>Barbed tubing plugs</t>
   </si>
   <si>
+    <t>1 pack</t>
+  </si>
+  <si>
     <t>https://www.mcmaster.com/5463K79-5463K791/</t>
   </si>
   <si>
@@ -785,7 +797,10 @@
     <t>5648K68-5648K681</t>
   </si>
   <si>
-    <t>3/32" ID tubing for sensor 25'</t>
+    <t>3/32" ID tubing for sensor</t>
+  </si>
+  <si>
+    <t>25ft</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/5648K68-5648K681/</t>
@@ -834,6 +849,24 @@
   </si>
   <si>
     <t>https://www.amazon.com/Converter-Supply-Module-Electronic-Transformer/dp/B01M9GBHBW/ref=sr_1_2_sspa?dchild=1&amp;keywords=12v+to+9v+dc+converter&amp;qid=1632698994&amp;sr=8-2-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzS05OT0dTSTRKSEwwJmVuY3J5cHRlZElkPUEwNTU4MDc0MTAzU0dUTEFDUlg4UCZlbmNyeXB0ZWRBZElkPUEwMDg5OTUyMUdCQlI1SENYRVFZTiZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=</t>
+  </si>
+  <si>
+    <t>46095K21</t>
+  </si>
+  <si>
+    <t>Diverting Valve</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/46095K21/</t>
+  </si>
+  <si>
+    <t>44705K36</t>
+  </si>
+  <si>
+    <t>1/8" Female-Female Connector</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/44705K36/</t>
   </si>
 </sst>
 </file>
@@ -845,7 +878,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="32">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -976,10 +1009,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
       <sz val="12.0"/>
       <color rgb="FF2D2926"/>
       <name val="Arial"/>
@@ -987,6 +1016,10 @@
     <font>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
     </font>
     <font>
       <color theme="1"/>
@@ -1189,25 +1222,25 @@
     <xf borderId="0" fillId="3" fontId="12" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="29" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="27" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="30" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="28" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1222,13 +1255,13 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="32" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -3793,20 +3826,20 @@
       <c r="D52" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="E52" s="50" t="s">
+      <c r="E52" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="F52" s="51">
+      <c r="F52" s="50">
         <v>10.16</v>
       </c>
-      <c r="G52" s="50">
-        <v>1.0</v>
+      <c r="G52" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I52" s="47" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J52" s="8">
         <v>10.16</v>
@@ -3834,22 +3867,22 @@
         <v>190</v>
       </c>
       <c r="D53" s="49" t="s">
-        <v>194</v>
-      </c>
-      <c r="E53" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="F53" s="52">
-        <v>15.05</v>
-      </c>
-      <c r="G53" s="50">
-        <v>1.0</v>
+      <c r="E53" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F53" s="50">
+        <v>3.01</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I53" s="47" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J53" s="8">
         <v>15.05</v>
@@ -3877,22 +3910,22 @@
         <v>190</v>
       </c>
       <c r="D54" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F54" s="50">
+        <v>2.82</v>
+      </c>
+      <c r="G54" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="E54" s="50" t="s">
-        <v>198</v>
-      </c>
-      <c r="F54" s="52">
-        <v>14.1</v>
-      </c>
-      <c r="G54" s="50">
-        <v>1.0</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J54" s="8">
         <v>14.1</v>
@@ -3920,12 +3953,12 @@
         <v>190</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F55" s="51">
+        <v>203</v>
+      </c>
+      <c r="F55" s="50">
         <v>0.55</v>
       </c>
       <c r="G55" s="10">
@@ -3935,7 +3968,7 @@
         <v>51</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="J55" s="8">
         <v>3.85</v>
@@ -3963,12 +3996,12 @@
         <v>190</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F56" s="51">
+        <v>206</v>
+      </c>
+      <c r="F56" s="50">
         <v>0.55</v>
       </c>
       <c r="G56" s="10">
@@ -3978,7 +4011,7 @@
         <v>51</v>
       </c>
       <c r="I56" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="J56" s="8">
         <v>1.1</v>
@@ -4006,22 +4039,22 @@
         <v>190</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="F57" s="51">
+        <v>209</v>
+      </c>
+      <c r="F57" s="50">
         <v>4.49</v>
       </c>
       <c r="G57" s="10">
         <v>2.0</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="I57" s="47" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J57" s="8">
         <v>8.98</v>
@@ -4048,23 +4081,23 @@
       <c r="C58" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D58" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="E58" s="50" t="s">
-        <v>211</v>
-      </c>
-      <c r="F58" s="52">
-        <v>29.2</v>
-      </c>
-      <c r="G58" s="50">
-        <v>1.0</v>
+      <c r="D58" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F58" s="50">
+        <v>2.92</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I58" s="24" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="J58" s="8">
         <v>29.2</v>
@@ -4091,23 +4124,23 @@
       <c r="C59" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D59" s="54" t="s">
-        <v>213</v>
+      <c r="D59" s="52" t="s">
+        <v>215</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F59" s="51">
+        <v>216</v>
+      </c>
+      <c r="F59" s="50">
         <v>83.95</v>
       </c>
       <c r="G59" s="10">
         <v>1.0</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="I59" s="47" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J59" s="8">
         <v>83.95</v>
@@ -4134,23 +4167,23 @@
       <c r="C60" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D60" s="55" t="s">
-        <v>217</v>
+      <c r="D60" s="53" t="s">
+        <v>219</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="F60" s="51">
+        <v>220</v>
+      </c>
+      <c r="F60" s="50">
         <v>123.86</v>
       </c>
       <c r="G60" s="10">
         <v>1.0</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="I60" s="47" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="J60" s="8">
         <v>123.86</v>
@@ -4177,23 +4210,23 @@
       <c r="C61" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D61" s="53" t="s">
-        <v>221</v>
+      <c r="D61" s="51" t="s">
+        <v>223</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="F61" s="51">
+        <v>224</v>
+      </c>
+      <c r="F61" s="50">
         <v>13.75</v>
       </c>
-      <c r="G61" s="50">
-        <v>2.0</v>
+      <c r="G61" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="J61" s="8">
         <v>27.5</v>
@@ -4220,13 +4253,13 @@
       <c r="C62" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D62" s="53" t="s">
-        <v>224</v>
+      <c r="D62" s="51" t="s">
+        <v>227</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="F62" s="51">
+        <v>228</v>
+      </c>
+      <c r="F62" s="50">
         <v>30.68</v>
       </c>
       <c r="G62" s="10">
@@ -4236,7 +4269,7 @@
         <v>51</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="J62" s="8">
         <v>30.68</v>
@@ -4263,13 +4296,13 @@
       <c r="C63" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D63" s="53" t="s">
-        <v>227</v>
+      <c r="D63" s="51" t="s">
+        <v>230</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="F63" s="51">
+        <v>231</v>
+      </c>
+      <c r="F63" s="50">
         <v>15.69</v>
       </c>
       <c r="G63" s="10">
@@ -4278,8 +4311,8 @@
       <c r="H63" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I63" s="47" t="s">
-        <v>229</v>
+      <c r="I63" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="J63" s="8">
         <v>15.69</v>
@@ -4306,13 +4339,13 @@
       <c r="C64" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D64" s="53" t="s">
-        <v>230</v>
+      <c r="D64" s="51" t="s">
+        <v>233</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="F64" s="51">
+        <v>234</v>
+      </c>
+      <c r="F64" s="50">
         <v>10.66</v>
       </c>
       <c r="G64" s="10">
@@ -4322,7 +4355,7 @@
         <v>51</v>
       </c>
       <c r="I64" s="24" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J64" s="8">
         <v>10.66</v>
@@ -4349,13 +4382,13 @@
       <c r="C65" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D65" s="53" t="s">
-        <v>233</v>
+      <c r="D65" s="51" t="s">
+        <v>236</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="F65" s="51">
+        <v>237</v>
+      </c>
+      <c r="F65" s="50">
         <v>14.73</v>
       </c>
       <c r="G65" s="10">
@@ -4365,7 +4398,7 @@
         <v>51</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="J65" s="8">
         <v>14.73</v>
@@ -4392,13 +4425,13 @@
       <c r="C66" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D66" s="53" t="s">
-        <v>236</v>
+      <c r="D66" s="51" t="s">
+        <v>239</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="F66" s="51">
+        <v>240</v>
+      </c>
+      <c r="F66" s="50">
         <v>1.03</v>
       </c>
       <c r="G66" s="10">
@@ -4408,7 +4441,7 @@
         <v>51</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J66" s="8">
         <v>1.03</v>
@@ -4435,13 +4468,13 @@
       <c r="C67" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D67" s="53" t="s">
-        <v>239</v>
+      <c r="D67" s="51" t="s">
+        <v>242</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F67" s="51">
+        <v>243</v>
+      </c>
+      <c r="F67" s="50">
         <v>8.95</v>
       </c>
       <c r="G67" s="10">
@@ -4451,7 +4484,7 @@
         <v>51</v>
       </c>
       <c r="I67" s="24" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="J67" s="8">
         <v>8.95</v>
@@ -4478,23 +4511,23 @@
       <c r="C68" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D68" s="53" t="s">
-        <v>242</v>
+      <c r="D68" s="51" t="s">
+        <v>245</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="F68" s="51">
+        <v>246</v>
+      </c>
+      <c r="F68" s="50">
         <v>9.14</v>
       </c>
-      <c r="G68" s="50">
-        <v>1.0</v>
+      <c r="G68" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="J68" s="8">
         <v>9.14</v>
@@ -4513,7 +4546,7 @@
     </row>
     <row r="69">
       <c r="A69" s="13">
-        <v>44465.0</v>
+        <v>44467.0</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>189</v>
@@ -4521,26 +4554,26 @@
       <c r="C69" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D69" s="53" t="s">
-        <v>245</v>
+      <c r="D69" s="51" t="s">
+        <v>249</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="F69" s="51">
+        <v>250</v>
+      </c>
+      <c r="F69" s="50">
         <v>2.87</v>
       </c>
-      <c r="G69" s="10">
-        <v>1.0</v>
+      <c r="G69" s="6">
+        <v>2.0</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I69" s="24" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="J69" s="8">
-        <v>2.87</v>
+        <v>5.74</v>
       </c>
       <c r="K69" s="10"/>
       <c r="L69" s="10"/>
@@ -4564,13 +4597,13 @@
       <c r="C70" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D70" s="53" t="s">
-        <v>248</v>
+      <c r="D70" s="51" t="s">
+        <v>252</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="F70" s="51">
+        <v>253</v>
+      </c>
+      <c r="F70" s="50">
         <v>5.79</v>
       </c>
       <c r="G70" s="10">
@@ -4580,7 +4613,7 @@
         <v>51</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="J70" s="8">
         <v>5.79</v>
@@ -4607,23 +4640,23 @@
       <c r="C71" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D71" s="56" t="s">
-        <v>251</v>
+      <c r="D71" s="54" t="s">
+        <v>255</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="F71" s="51">
+        <v>256</v>
+      </c>
+      <c r="F71" s="50">
         <v>19.51</v>
       </c>
       <c r="G71" s="10">
         <v>1.0</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="I71" s="47" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="J71" s="8">
         <v>19.51</v>
@@ -4650,23 +4683,23 @@
       <c r="C72" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D72" s="53" t="s">
-        <v>255</v>
-      </c>
-      <c r="E72" s="50" t="s">
-        <v>256</v>
-      </c>
-      <c r="F72" s="52">
-        <v>6.75</v>
-      </c>
-      <c r="G72" s="50">
-        <v>1.0</v>
+      <c r="D72" s="51" t="s">
+        <v>259</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F72" s="50">
+        <v>0.27</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="J72" s="8">
         <v>6.75</v>
@@ -4693,13 +4726,13 @@
       <c r="C73" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D73" s="53" t="s">
-        <v>258</v>
+      <c r="D73" s="51" t="s">
+        <v>263</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F73" s="51">
+        <v>264</v>
+      </c>
+      <c r="F73" s="50">
         <v>6.93</v>
       </c>
       <c r="G73" s="10">
@@ -4709,7 +4742,7 @@
         <v>51</v>
       </c>
       <c r="I73" s="24" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="J73" s="8">
         <v>6.93</v>
@@ -4736,13 +4769,13 @@
       <c r="C74" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D74" s="53" t="s">
-        <v>261</v>
+      <c r="D74" s="51" t="s">
+        <v>266</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="F74" s="51">
+        <v>267</v>
+      </c>
+      <c r="F74" s="50">
         <v>5.38</v>
       </c>
       <c r="G74" s="10">
@@ -4752,7 +4785,7 @@
         <v>51</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="J74" s="8">
         <v>10.76</v>
@@ -4779,13 +4812,13 @@
       <c r="C75" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D75" s="53" t="s">
-        <v>264</v>
+      <c r="D75" s="51" t="s">
+        <v>269</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="F75" s="51">
+        <v>270</v>
+      </c>
+      <c r="F75" s="50">
         <v>14.07</v>
       </c>
       <c r="G75" s="10">
@@ -4795,7 +4828,7 @@
         <v>51</v>
       </c>
       <c r="I75" s="24" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="J75" s="8">
         <v>14.07</v>
@@ -4822,13 +4855,13 @@
       <c r="C76" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D76" s="53" t="s">
-        <v>267</v>
+      <c r="D76" s="51" t="s">
+        <v>272</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="F76" s="51">
+        <v>273</v>
+      </c>
+      <c r="F76" s="50">
         <v>8.14</v>
       </c>
       <c r="G76" s="10">
@@ -4838,7 +4871,7 @@
         <v>51</v>
       </c>
       <c r="I76" s="24" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="J76" s="8">
         <v>8.14</v>
@@ -4865,13 +4898,13 @@
       <c r="C77" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D77" s="55" t="s">
-        <v>270</v>
+      <c r="D77" s="53" t="s">
+        <v>275</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="F77" s="51">
+        <v>276</v>
+      </c>
+      <c r="F77" s="50">
         <v>7.59</v>
       </c>
       <c r="G77" s="10">
@@ -4881,7 +4914,7 @@
         <v>19</v>
       </c>
       <c r="I77" s="47" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="J77" s="8">
         <v>7.59</v>
@@ -4899,35 +4932,79 @@
       <c r="Q77" s="10"/>
     </row>
     <row r="78">
-      <c r="A78" s="48"/>
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="10"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="47"/>
-      <c r="J78" s="32"/>
+      <c r="A78" s="13">
+        <v>44467.0</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D78" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="F78" s="8">
+        <v>25.03</v>
+      </c>
+      <c r="G78" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I78" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="J78" s="8">
+        <v>25.03</v>
+      </c>
       <c r="K78" s="10"/>
       <c r="L78" s="10"/>
-      <c r="M78" s="11"/>
-      <c r="N78" s="11"/>
+      <c r="M78" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N78" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="O78" s="17"/>
       <c r="P78" s="12"/>
       <c r="Q78" s="10"/>
     </row>
     <row r="79">
-      <c r="A79" s="12"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="32"/>
-      <c r="G79" s="10"/>
-      <c r="H79" s="10"/>
-      <c r="I79" s="47"/>
-      <c r="J79" s="32"/>
+      <c r="A79" s="13">
+        <v>44467.0</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="F79" s="8">
+        <v>2.46</v>
+      </c>
+      <c r="G79" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I79" s="56" t="s">
+        <v>283</v>
+      </c>
+      <c r="J79" s="8">
+        <v>2.46</v>
+      </c>
       <c r="K79" s="10"/>
       <c r="L79" s="10"/>
       <c r="M79" s="57"/>
@@ -9720,7 +9797,9 @@
     <hyperlink r:id="rId71" ref="I75"/>
     <hyperlink r:id="rId72" ref="I76"/>
     <hyperlink r:id="rId73" ref="I77"/>
+    <hyperlink r:id="rId74" ref="I78"/>
+    <hyperlink r:id="rId75" ref="I79"/>
   </hyperlinks>
-  <drawing r:id="rId74"/>
+  <drawing r:id="rId76"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a link section to parts. Create a dict for links.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,15 +5,13 @@
   <sheets>
     <sheet state="visible" name="Purchasing List" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Purchasing List'!$A$1:$P$3</definedName>
-  </definedNames>
+  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="280">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -442,6 +440,9 @@
     <t>https://www.amazon.com/gp/product/B003Q6CB70/ref=ox_sc_saved_title_2?smid=ATVPDKIKX0DER&amp;psc=1</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>B07ZBNCKMS</t>
   </si>
   <si>
@@ -593,10 +594,7 @@
     <t>9284K616</t>
   </si>
   <si>
-    <t>Polyester Expandable Sleeving</t>
-  </si>
-  <si>
-    <t>10ft</t>
+    <t>Polyester Expandable Sleeving 10ft</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/9284K616-9284K364/</t>
@@ -605,10 +603,7 @@
     <t>5549K37</t>
   </si>
   <si>
-    <t>Abrasion-Resistant Versilon Polyurethane Tubing</t>
-  </si>
-  <si>
-    <t>5ft</t>
+    <t>Abrasion-Resistant Versilon Polyurethane Tubing 5ft</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/5549K37/</t>
@@ -617,7 +612,7 @@
     <t>5234K52-5234K82</t>
   </si>
   <si>
-    <t>Super-Soft Latex Rubber Tubing for Air&amp;Water</t>
+    <t>Super-Soft Latex Rubber Tubing for Air&amp;Water 5ft</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/5234K52-5234K82/</t>
@@ -656,7 +651,7 @@
     <t>5108K58</t>
   </si>
   <si>
-    <t>Abrasion-Resistant Polyurethane Tube for Air</t>
+    <t>Abrasion-Resistant Polyurethane Tube for Air 10ft</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/5108K58/</t>
@@ -692,9 +687,6 @@
     <t>Worm Drive Clamps</t>
   </si>
   <si>
-    <t>2 packs</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/5011T171/</t>
   </si>
   <si>
@@ -758,9 +750,6 @@
     <t>Barbed tubing plugs</t>
   </si>
   <si>
-    <t>1 pack</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/5463K79-5463K791/</t>
   </si>
   <si>
@@ -797,10 +786,7 @@
     <t>5648K68-5648K681</t>
   </si>
   <si>
-    <t>3/32" ID tubing for sensor</t>
-  </si>
-  <si>
-    <t>25ft</t>
+    <t>3/32" ID tubing for sensor 25ft</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/5648K68-5648K681/</t>
@@ -1527,7 +1513,7 @@
     <col customWidth="1" min="16" max="16" width="17.0"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="24.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1578,7 +1564,7 @@
       </c>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" hidden="1">
+    <row r="2">
       <c r="A2" s="5">
         <v>44450.0</v>
       </c>
@@ -1613,12 +1599,14 @@
       <c r="M2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="12"/>
+      <c r="N2" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" hidden="1">
+    <row r="3">
       <c r="A3" s="13">
         <v>44453.0</v>
       </c>
@@ -1655,7 +1643,9 @@
       <c r="M3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="17"/>
+      <c r="N3" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
       <c r="Q3" s="4"/>
@@ -3240,7 +3230,7 @@
         <v>21</v>
       </c>
       <c r="N38" s="11" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="O38" s="23"/>
       <c r="P38" s="12"/>
@@ -3257,10 +3247,10 @@
         <v>23</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F39" s="8">
         <v>7.99</v>
@@ -3272,7 +3262,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J39" s="8">
         <v>7.99</v>
@@ -3302,10 +3292,10 @@
         <v>23</v>
       </c>
       <c r="D40" s="43" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F40" s="8">
         <v>83.89</v>
@@ -3317,13 +3307,13 @@
         <v>51</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J40" s="8">
         <v>83.89</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L40" s="16" t="s">
         <v>26</v>
@@ -3349,10 +3339,10 @@
         <v>23</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E41" s="46" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F41" s="8">
         <v>39.42</v>
@@ -3364,13 +3354,13 @@
         <v>51</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J41" s="8">
         <v>39.42</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L41" s="16" t="s">
         <v>26</v>
@@ -3396,10 +3386,10 @@
         <v>23</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E42" s="46" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F42" s="8">
         <v>4.41</v>
@@ -3408,10 +3398,10 @@
         <v>1.0</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J42" s="8">
         <v>4.41</v>
@@ -3442,7 +3432,7 @@
       </c>
       <c r="D43" s="46"/>
       <c r="E43" s="46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F43" s="8">
         <v>20.0</v>
@@ -3451,14 +3441,14 @@
         <v>1.0</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I43" s="47"/>
       <c r="J43" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L43" s="16" t="s">
         <v>26</v>
@@ -3485,7 +3475,7 @@
       </c>
       <c r="D44" s="46"/>
       <c r="E44" s="46" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F44" s="8">
         <v>5.0</v>
@@ -3494,11 +3484,11 @@
         <v>3.0</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I44" s="47"/>
       <c r="J44" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" s="16" t="s">
@@ -3526,7 +3516,7 @@
       </c>
       <c r="D45" s="46"/>
       <c r="E45" s="46" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F45" s="8">
         <v>0.1</v>
@@ -3535,14 +3525,14 @@
         <v>1.0</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I45" s="47"/>
       <c r="J45" s="8">
         <v>0.1</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L45" s="16" t="s">
         <v>26</v>
@@ -3562,16 +3552,16 @@
         <v>44464.0</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F46" s="8">
         <v>74.9</v>
@@ -3583,16 +3573,18 @@
         <v>19</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J46" s="32"/>
       <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
+      <c r="L46" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M46" s="11" t="s">
         <v>21</v>
       </c>
       <c r="N46" s="11" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="O46" s="23"/>
       <c r="P46" s="12"/>
@@ -3603,16 +3595,16 @@
         <v>44464.0</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D47" s="44">
         <v>638358.0</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F47" s="8">
         <v>14.99</v>
@@ -3624,13 +3616,15 @@
         <v>117</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J47" s="8">
         <v>14.99</v>
       </c>
       <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
+      <c r="L47" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M47" s="11" t="s">
         <v>21</v>
       </c>
@@ -3646,16 +3640,16 @@
         <v>44464.0</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F48" s="8">
         <v>27.49</v>
@@ -3667,13 +3661,15 @@
         <v>19</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J48" s="8">
         <v>27.49</v>
       </c>
       <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
+      <c r="L48" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M48" s="11" t="s">
         <v>21</v>
       </c>
@@ -3689,16 +3685,16 @@
         <v>44464.0</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E49" s="46" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F49" s="8">
         <v>19.99</v>
@@ -3710,13 +3706,15 @@
         <v>19</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J49" s="8">
         <v>19.99</v>
       </c>
       <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
+      <c r="L49" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M49" s="11" t="s">
         <v>21</v>
       </c>
@@ -3729,19 +3727,19 @@
     </row>
     <row r="50">
       <c r="A50" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D50" s="30">
         <v>856.0</v>
       </c>
       <c r="E50" s="46" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F50" s="8">
         <v>3.75</v>
@@ -3753,14 +3751,16 @@
         <v>73</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J50" s="32">
         <f t="shared" ref="J50:J51" si="2">F50*G50</f>
         <v>7.5</v>
       </c>
       <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
+      <c r="L50" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M50" s="11" t="s">
         <v>21</v>
       </c>
@@ -3774,16 +3774,16 @@
     <row r="51">
       <c r="A51" s="12"/>
       <c r="B51" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E51" s="46" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F51" s="8">
         <v>4.99</v>
@@ -3795,14 +3795,16 @@
         <v>19</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J51" s="32">
         <f t="shared" si="2"/>
         <v>9.98</v>
       </c>
       <c r="K51" s="10"/>
-      <c r="L51" s="10"/>
+      <c r="L51" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M51" s="11" t="s">
         <v>21</v>
       </c>
@@ -3818,22 +3820,22 @@
         <v>44465.0</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D52" s="49" t="s">
-        <v>191</v>
-      </c>
-      <c r="E52" s="4" t="s">
         <v>192</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="F52" s="50">
         <v>10.16</v>
       </c>
-      <c r="G52" s="4" t="s">
-        <v>193</v>
+      <c r="G52" s="7">
+        <v>1.0</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>51</v>
@@ -3845,7 +3847,9 @@
         <v>10.16</v>
       </c>
       <c r="K52" s="10"/>
-      <c r="L52" s="10"/>
+      <c r="L52" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M52" s="11" t="s">
         <v>21</v>
       </c>
@@ -3861,34 +3865,36 @@
         <v>44465.0</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D53" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="7" t="s">
         <v>196</v>
       </c>
       <c r="F53" s="50">
-        <v>3.01</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>197</v>
+        <v>15.05</v>
+      </c>
+      <c r="G53" s="7">
+        <v>1.0</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I53" s="47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J53" s="8">
         <v>15.05</v>
       </c>
       <c r="K53" s="10"/>
-      <c r="L53" s="10"/>
+      <c r="L53" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M53" s="11" t="s">
         <v>21</v>
       </c>
@@ -3904,34 +3910,36 @@
         <v>44465.0</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D54" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="F54" s="50">
-        <v>2.82</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>197</v>
+        <v>14.1</v>
+      </c>
+      <c r="G54" s="7">
+        <v>1.0</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J54" s="8">
         <v>14.1</v>
       </c>
       <c r="K54" s="10"/>
-      <c r="L54" s="10"/>
+      <c r="L54" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M54" s="11" t="s">
         <v>21</v>
       </c>
@@ -3947,16 +3955,16 @@
         <v>44465.0</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D55" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>203</v>
       </c>
       <c r="F55" s="50">
         <v>0.55</v>
@@ -3968,13 +3976,15 @@
         <v>51</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J55" s="8">
         <v>3.85</v>
       </c>
       <c r="K55" s="10"/>
-      <c r="L55" s="10"/>
+      <c r="L55" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M55" s="11" t="s">
         <v>21</v>
       </c>
@@ -3990,16 +4000,16 @@
         <v>44465.0</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D56" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="F56" s="50">
         <v>0.55</v>
@@ -4011,13 +4021,15 @@
         <v>51</v>
       </c>
       <c r="I56" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J56" s="8">
         <v>1.1</v>
       </c>
       <c r="K56" s="4"/>
-      <c r="L56" s="10"/>
+      <c r="L56" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M56" s="11" t="s">
         <v>21</v>
       </c>
@@ -4033,16 +4045,16 @@
         <v>44465.0</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D57" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>209</v>
       </c>
       <c r="F57" s="50">
         <v>4.49</v>
@@ -4051,16 +4063,18 @@
         <v>2.0</v>
       </c>
       <c r="H57" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="I57" s="47" t="s">
         <v>210</v>
-      </c>
-      <c r="I57" s="47" t="s">
-        <v>211</v>
       </c>
       <c r="J57" s="8">
         <v>8.98</v>
       </c>
       <c r="K57" s="10"/>
-      <c r="L57" s="10"/>
+      <c r="L57" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M57" s="11" t="s">
         <v>21</v>
       </c>
@@ -4076,34 +4090,36 @@
         <v>44465.0</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D58" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>213</v>
-      </c>
       <c r="F58" s="50">
-        <v>2.92</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>193</v>
+        <v>29.2</v>
+      </c>
+      <c r="G58" s="7">
+        <v>1.0</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I58" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J58" s="8">
         <v>29.2</v>
       </c>
       <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
+      <c r="L58" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M58" s="11" t="s">
         <v>21</v>
       </c>
@@ -4119,16 +4135,16 @@
         <v>44465.0</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D59" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="E59" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="F59" s="50">
         <v>83.95</v>
@@ -4137,16 +4153,18 @@
         <v>1.0</v>
       </c>
       <c r="H59" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="I59" s="47" t="s">
         <v>217</v>
-      </c>
-      <c r="I59" s="47" t="s">
-        <v>218</v>
       </c>
       <c r="J59" s="8">
         <v>83.95</v>
       </c>
       <c r="K59" s="10"/>
-      <c r="L59" s="10"/>
+      <c r="L59" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M59" s="11" t="s">
         <v>21</v>
       </c>
@@ -4162,16 +4180,16 @@
         <v>44465.0</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D60" s="53" t="s">
+        <v>218</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>219</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>220</v>
       </c>
       <c r="F60" s="50">
         <v>123.86</v>
@@ -4180,16 +4198,18 @@
         <v>1.0</v>
       </c>
       <c r="H60" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="I60" s="47" t="s">
         <v>221</v>
-      </c>
-      <c r="I60" s="47" t="s">
-        <v>222</v>
       </c>
       <c r="J60" s="8">
         <v>123.86</v>
       </c>
       <c r="K60" s="10"/>
-      <c r="L60" s="10"/>
+      <c r="L60" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M60" s="11" t="s">
         <v>21</v>
       </c>
@@ -4205,34 +4225,36 @@
         <v>44465.0</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D61" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>224</v>
       </c>
       <c r="F61" s="50">
         <v>13.75</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>225</v>
+      <c r="G61" s="7">
+        <v>2.0</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J61" s="8">
         <v>27.5</v>
       </c>
       <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
+      <c r="L61" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M61" s="11" t="s">
         <v>21</v>
       </c>
@@ -4248,16 +4270,16 @@
         <v>44465.0</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D62" s="51" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F62" s="50">
         <v>30.68</v>
@@ -4269,13 +4291,15 @@
         <v>51</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J62" s="8">
         <v>30.68</v>
       </c>
       <c r="K62" s="10"/>
-      <c r="L62" s="10"/>
+      <c r="L62" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M62" s="11" t="s">
         <v>21</v>
       </c>
@@ -4291,16 +4315,16 @@
         <v>44465.0</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D63" s="51" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F63" s="50">
         <v>15.69</v>
@@ -4312,13 +4336,15 @@
         <v>19</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J63" s="8">
         <v>15.69</v>
       </c>
       <c r="K63" s="10"/>
-      <c r="L63" s="10"/>
+      <c r="L63" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M63" s="11" t="s">
         <v>21</v>
       </c>
@@ -4334,16 +4360,16 @@
         <v>44465.0</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D64" s="51" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F64" s="50">
         <v>10.66</v>
@@ -4355,13 +4381,15 @@
         <v>51</v>
       </c>
       <c r="I64" s="24" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J64" s="8">
         <v>10.66</v>
       </c>
       <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
+      <c r="L64" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M64" s="11" t="s">
         <v>21</v>
       </c>
@@ -4377,16 +4405,16 @@
         <v>44465.0</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D65" s="51" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F65" s="50">
         <v>14.73</v>
@@ -4398,13 +4426,15 @@
         <v>51</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J65" s="8">
         <v>14.73</v>
       </c>
       <c r="K65" s="10"/>
-      <c r="L65" s="10"/>
+      <c r="L65" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M65" s="11" t="s">
         <v>21</v>
       </c>
@@ -4420,16 +4450,16 @@
         <v>44465.0</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D66" s="51" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F66" s="50">
         <v>1.03</v>
@@ -4441,13 +4471,15 @@
         <v>51</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J66" s="8">
         <v>1.03</v>
       </c>
       <c r="K66" s="10"/>
-      <c r="L66" s="10"/>
+      <c r="L66" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M66" s="11" t="s">
         <v>21</v>
       </c>
@@ -4463,16 +4495,16 @@
         <v>44465.0</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D67" s="51" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F67" s="50">
         <v>8.95</v>
@@ -4484,13 +4516,15 @@
         <v>51</v>
       </c>
       <c r="I67" s="24" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J67" s="8">
         <v>8.95</v>
       </c>
       <c r="K67" s="10"/>
-      <c r="L67" s="10"/>
+      <c r="L67" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M67" s="11" t="s">
         <v>21</v>
       </c>
@@ -4506,34 +4540,36 @@
         <v>44465.0</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D68" s="51" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F68" s="50">
         <v>9.14</v>
       </c>
-      <c r="G68" s="4" t="s">
-        <v>247</v>
+      <c r="G68" s="7">
+        <v>1.0</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="J68" s="8">
         <v>9.14</v>
       </c>
       <c r="K68" s="10"/>
-      <c r="L68" s="10"/>
+      <c r="L68" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M68" s="11" t="s">
         <v>21</v>
       </c>
@@ -4549,16 +4585,16 @@
         <v>44467.0</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D69" s="51" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F69" s="50">
         <v>2.87</v>
@@ -4570,13 +4606,15 @@
         <v>51</v>
       </c>
       <c r="I69" s="24" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J69" s="8">
         <v>5.74</v>
       </c>
       <c r="K69" s="10"/>
-      <c r="L69" s="10"/>
+      <c r="L69" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M69" s="11" t="s">
         <v>21</v>
       </c>
@@ -4592,16 +4630,16 @@
         <v>44465.0</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D70" s="51" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F70" s="50">
         <v>5.79</v>
@@ -4613,13 +4651,15 @@
         <v>51</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J70" s="8">
         <v>5.79</v>
       </c>
       <c r="K70" s="10"/>
-      <c r="L70" s="10"/>
+      <c r="L70" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M70" s="11" t="s">
         <v>21</v>
       </c>
@@ -4635,16 +4675,16 @@
         <v>44465.0</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D71" s="54" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F71" s="50">
         <v>19.51</v>
@@ -4653,16 +4693,18 @@
         <v>1.0</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="I71" s="47" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J71" s="8">
         <v>19.51</v>
       </c>
       <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
+      <c r="L71" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M71" s="11" t="s">
         <v>21</v>
       </c>
@@ -4678,34 +4720,36 @@
         <v>44465.0</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D72" s="51" t="s">
-        <v>259</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>257</v>
       </c>
       <c r="F72" s="50">
-        <v>0.27</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>261</v>
+        <v>6.75</v>
+      </c>
+      <c r="G72" s="7">
+        <v>1.0</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="J72" s="8">
         <v>6.75</v>
       </c>
       <c r="K72" s="10"/>
-      <c r="L72" s="10"/>
+      <c r="L72" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M72" s="11" t="s">
         <v>21</v>
       </c>
@@ -4721,16 +4765,16 @@
         <v>44465.0</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D73" s="51" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F73" s="50">
         <v>6.93</v>
@@ -4742,13 +4786,15 @@
         <v>51</v>
       </c>
       <c r="I73" s="24" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="J73" s="8">
         <v>6.93</v>
       </c>
       <c r="K73" s="10"/>
-      <c r="L73" s="10"/>
+      <c r="L73" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M73" s="11" t="s">
         <v>21</v>
       </c>
@@ -4764,16 +4810,16 @@
         <v>44465.0</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D74" s="51" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F74" s="50">
         <v>5.38</v>
@@ -4785,13 +4831,15 @@
         <v>51</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J74" s="8">
         <v>10.76</v>
       </c>
       <c r="K74" s="10"/>
-      <c r="L74" s="10"/>
+      <c r="L74" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M74" s="11" t="s">
         <v>21</v>
       </c>
@@ -4807,16 +4855,16 @@
         <v>44465.0</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D75" s="51" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F75" s="50">
         <v>14.07</v>
@@ -4828,13 +4876,15 @@
         <v>51</v>
       </c>
       <c r="I75" s="24" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="J75" s="8">
         <v>14.07</v>
       </c>
       <c r="K75" s="10"/>
-      <c r="L75" s="10"/>
+      <c r="L75" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M75" s="11" t="s">
         <v>21</v>
       </c>
@@ -4850,16 +4900,16 @@
         <v>44465.0</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D76" s="51" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F76" s="50">
         <v>8.14</v>
@@ -4871,13 +4921,15 @@
         <v>51</v>
       </c>
       <c r="I76" s="24" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="J76" s="8">
         <v>8.14</v>
       </c>
       <c r="K76" s="10"/>
-      <c r="L76" s="10"/>
+      <c r="L76" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M76" s="11" t="s">
         <v>21</v>
       </c>
@@ -4893,16 +4945,16 @@
         <v>44465.0</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D77" s="53" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F77" s="50">
         <v>7.59</v>
@@ -4914,13 +4966,15 @@
         <v>19</v>
       </c>
       <c r="I77" s="47" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="J77" s="8">
         <v>7.59</v>
       </c>
       <c r="K77" s="10"/>
-      <c r="L77" s="10"/>
+      <c r="L77" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M77" s="11" t="s">
         <v>21</v>
       </c>
@@ -4936,16 +4990,16 @@
         <v>44467.0</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D78" s="55" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F78" s="8">
         <v>25.03</v>
@@ -4957,13 +5011,15 @@
         <v>51</v>
       </c>
       <c r="I78" s="56" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="J78" s="8">
         <v>25.03</v>
       </c>
       <c r="K78" s="10"/>
-      <c r="L78" s="10"/>
+      <c r="L78" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M78" s="11" t="s">
         <v>21</v>
       </c>
@@ -4979,16 +5035,16 @@
         <v>44467.0</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F79" s="8">
         <v>2.46</v>
@@ -5000,13 +5056,15 @@
         <v>51</v>
       </c>
       <c r="I79" s="56" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="J79" s="8">
         <v>2.46</v>
       </c>
       <c r="K79" s="10"/>
-      <c r="L79" s="10"/>
+      <c r="L79" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="M79" s="57"/>
       <c r="N79" s="57"/>
       <c r="O79" s="17"/>
@@ -9703,23 +9761,18 @@
       <c r="N1000" s="66"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$P$3">
-    <filterColumn colId="12">
-      <filters/>
-    </filterColumn>
-  </autoFilter>
-  <conditionalFormatting sqref="M1:M1000 N1 N4:N1000">
+  <conditionalFormatting sqref="M1:N1000">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1000 N1 N4:N1000">
+  <conditionalFormatting sqref="M1:N1000">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="M2:M3 M4:N1000">
+    <dataValidation type="list" allowBlank="1" sqref="M2:N1000">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>